<commit_message>
Fixed missing time period
</commit_message>
<xml_diff>
--- a/Templates/Monthly Billable Hours Report.xlsx
+++ b/Templates/Monthly Billable Hours Report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Repos\PowerShell\Modules\Toggl.Functions\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E75F169-A251-4C4C-B2E3-38F7BE6B692C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDDE2CE-1235-4AC6-91C3-A585340694DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19860" windowHeight="10350" activeTab="1" xr2:uid="{A3BC51AE-B274-46BE-8E18-D8AD58958BB1}"/>
   </bookViews>
@@ -257,19 +257,19 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$2:$B$12</c:f>
+              <c:f>Data!$B$2:$B$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -334,19 +334,19 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$2:$C$12</c:f>
+              <c:f>Data!$C$2:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -411,19 +411,19 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$2:$D$12</c:f>
+              <c:f>Data!$D$2:$D$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -512,13 +512,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Data!$A$2:$A$12</c15:sqref>
+                          <c15:sqref>Data!$A$2:$A$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>mmm\-yy</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                     </c:numCache>
                   </c:numRef>
                 </c:cat>
@@ -527,13 +527,13 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Data!$E$2:$E$12</c15:sqref>
+                          <c15:sqref>Data!$E$2:$E$13</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="11"/>
+                      <c:ptCount val="12"/>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
@@ -603,51 +603,54 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$A$2:$A$12</c:f>
+              <c:f>Data!$A$2:$A$13</c:f>
               <c:numCache>
                 <c:formatCode>mmm\-yy</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$F$2:$F$12</c:f>
+              <c:f>Data!$F$2:$F$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>110</c:v>
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>160</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1797,10 +1800,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C1690A-F13F-46FB-9B46-80139F0EA332}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1836,71 +1839,77 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="F2">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="F3">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="F4">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="F5">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="F6">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="F7">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="F8">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="F9">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="F10">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="F11">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="F12">
-        <v>110</v>
+        <v>160</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="F13">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update report to include target
!deploy
</commit_message>
<xml_diff>
--- a/Templates/Monthly Billable Hours Report.xlsx
+++ b/Templates/Monthly Billable Hours Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Repos\PowerShell\Modules\Toggl.Functions\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDDE2CE-1235-4AC6-91C3-A585340694DA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AF64FD-FEC1-4161-9E5D-C627CC42BF11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19860" windowHeight="10350" activeTab="1" xr2:uid="{A3BC51AE-B274-46BE-8E18-D8AD58958BB1}"/>
   </bookViews>
@@ -48,10 +48,10 @@
     <t>Total(hrs)</t>
   </si>
   <si>
-    <t>Target</t>
+    <t>Target(hrs)</t>
   </si>
   <si>
-    <t>Get-TogglMonthlyHoursReport | ConvertTo-Csv -NoTypeInformation -Delimiter "`t" | clip</t>
+    <t>Get-TogglMonthlyHoursReport | ConvertTo-Csv -NoTypeInformation -Delimiter "`t" | select -Skip 1 | clip</t>
   </si>
 </sst>
 </file>
@@ -559,7 +559,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Target</c:v>
+                  <c:v>Target(hrs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -616,42 +616,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>160</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>160</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1813,7 +1777,7 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1838,75 +1802,39 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="F2">
-        <v>160</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="F3">
-        <v>160</v>
-      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="F4">
-        <v>160</v>
-      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="F5">
-        <v>160</v>
-      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="F6">
-        <v>160</v>
-      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="F7">
-        <v>160</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="F8">
-        <v>160</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="F9">
-        <v>160</v>
-      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="F10">
-        <v>160</v>
-      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="F11">
-        <v>160</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="F12">
-        <v>160</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="F13">
-        <v>160</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Update monthly billable hours report template
</commit_message>
<xml_diff>
--- a/Templates/Monthly Billable Hours Report.xlsx
+++ b/Templates/Monthly Billable Hours Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Repos\PowerShell\Modules\Toggl.Functions\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AF64FD-FEC1-4161-9E5D-C627CC42BF11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191D88EB-D899-4CB9-AC95-D22C44FA2F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19860" windowHeight="10350" activeTab="1" xr2:uid="{A3BC51AE-B274-46BE-8E18-D8AD58958BB1}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Chart" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
     <t>Total(hrs)</t>
   </si>
   <si>
-    <t>Target(hrs)</t>
+    <t>Target</t>
   </si>
   <si>
     <t>Get-TogglMonthlyHoursReport | ConvertTo-Csv -NoTypeInformation -Delimiter "`t" | select -Skip 1 | clip</t>
@@ -93,10 +93,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,7 +554,7 @@
         </c:extLst>
       </c:barChart>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="4"/>
@@ -559,7 +565,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Target(hrs)</c:v>
+                  <c:v>Target</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -567,7 +573,9 @@
           <c:spPr>
             <a:ln w="34925" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -588,7 +596,9 @@
               </a:solidFill>
               <a:ln w="9525">
                 <a:solidFill>
-                  <a:schemeClr val="accent6"/>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="50000"/>
+                  </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -619,10 +629,362 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-BF25-4FC2-AD81-05E1FB58D932}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>90%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$G$2:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-E132-480A-BA60-D284AC648A3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>80%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="60000"/>
+                    <a:lumOff val="40000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$H$2:$H$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E132-480A-BA60-D284AC648A3B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>70%</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="40000"/>
+                  <a:lumOff val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$13</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yy</c:formatCode>
+                <c:ptCount val="12"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Data!$I$2:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E132-480A-BA60-D284AC648A3B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1764,7 +2126,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C1690A-F13F-46FB-9B46-80139F0EA332}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
@@ -1772,71 +2134,225 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="H1" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="I1" s="4">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
+      <c r="G2">
+        <f>F2*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <f>F2*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f>F2*0.7</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
+      <c r="G3">
+        <f>F3*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>F3*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I13" si="0">F3*0.7</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
+      <c r="G4">
+        <f>F4*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>F4*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
+      <c r="G5">
+        <f>F5*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>F5*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
+      <c r="G6">
+        <f>F6*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>F6*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
+      <c r="G7">
+        <f>F7*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>F7*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
+      <c r="G8">
+        <f>F8*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>F8*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
+      <c r="G9">
+        <f>F9*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>F9*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
+      <c r="G10">
+        <f>F10*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>F10*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
+      <c r="G11">
+        <f>F11*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>F11*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
+      <c r="G12">
+        <f>F12*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>F12*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
+      <c r="G13">
+        <f>F13*0.9</f>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f>F13*0.8</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Update monthly hours report to include multiple target percentages
!deploy
</commit_message>
<xml_diff>
--- a/Templates/Monthly Billable Hours Report.xlsx
+++ b/Templates/Monthly Billable Hours Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Repos\PowerShell\Modules\Toggl.Functions\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191D88EB-D899-4CB9-AC95-D22C44FA2F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4CE12A-618A-48EC-8992-A8EFD07B5320}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19860" windowHeight="10350" activeTab="1" xr2:uid="{A3BC51AE-B274-46BE-8E18-D8AD58958BB1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Month</t>
   </si>
@@ -48,10 +48,19 @@
     <t>Total(hrs)</t>
   </si>
   <si>
-    <t>Target</t>
+    <t>Get-TogglMonthlyHoursReport | ConvertTo-Csv -NoTypeInformation -Delimiter "`t" | select -Skip 1 | clip</t>
   </si>
   <si>
-    <t>Get-TogglMonthlyHoursReport | ConvertTo-Csv -NoTypeInformation -Delimiter "`t" | select -Skip 1 | clip</t>
+    <t>Target(100%)</t>
+  </si>
+  <si>
+    <t>Target(90%)</t>
+  </si>
+  <si>
+    <t>Target(80%)</t>
+  </si>
+  <si>
+    <t>Target(70%)</t>
   </si>
 </sst>
 </file>
@@ -93,14 +102,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -565,7 +571,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Target</c:v>
+                  <c:v>Target(100%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -645,7 +651,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>90%</c:v>
+                  <c:v>Target(90%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -706,42 +712,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -761,7 +731,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>80%</c:v>
+                  <c:v>Target(80%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -824,42 +794,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -879,7 +813,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>70%</c:v>
+                  <c:v>Target(70%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -942,42 +876,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2139,8 +2037,8 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2160,201 +2058,57 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
-      <c r="G1" s="4">
-        <v>0.9</v>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
       </c>
-      <c r="H1" s="4">
-        <v>0.8</v>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
       </c>
-      <c r="I1" s="4">
-        <v>0.7</v>
+      <c r="I1" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="G2">
-        <f>F2*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <f>F2*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <f>F2*0.7</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="G3">
-        <f>F3*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <f>F3*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I13" si="0">F3*0.7</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="G4">
-        <f>F4*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <f>F4*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="G5">
-        <f>F5*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <f>F5*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="G6">
-        <f>F6*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <f>F6*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="G7">
-        <f>F7*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <f>F7*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="G8">
-        <f>F8*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <f>F8*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="G9">
-        <f>F9*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <f>F9*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="G10">
-        <f>F10*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <f>F10*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="G11">
-        <f>F11*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <f>F11*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="G12">
-        <f>F12*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <f>F12*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="G13">
-        <f>F13*0.9</f>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f>F13*0.8</f>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>